<commit_message>
Product backlog for user and developer
</commit_message>
<xml_diff>
--- a/Product-backlog.xlsx
+++ b/Product-backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://habibuniversity-my.sharepoint.com/personal/shariq_raees_habib_edu_pk/Documents/Documents/GitHub/PROG5001A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_534B820E1C5E093D0E6E77DE570509F5B34C871A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{84597D30-4643-44CE-A670-C3BC74FEF59D}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_534B820E1C5E093D0E6E77DE570509F5B34C871A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8718E85-53EB-464C-BDBF-AB4EC0ECB47A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Week 9</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>to close the game when finised</t>
+  </si>
+  <si>
+    <t>class converted to abstract due to some new abstract methods.</t>
   </si>
 </sst>
 </file>
@@ -658,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,10 +878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,11 +1093,10 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
+      <c r="C14" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="2"/>
       <c r="G14" s="34"/>
@@ -1105,10 +1107,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
-      <c r="B15" s="6"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="G15" s="34"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1118,8 +1121,9 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="6"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="34"/>
       <c r="H16" s="6"/>
@@ -1130,21 +1134,20 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="6"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="34"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>3.2</v>
-      </c>
+      <c r="A18" s="12"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1152,12 +1155,12 @@
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>31</v>
+      <c r="A19" s="11">
+        <v>3.2</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="D19" s="5" t="s">
-        <v>25</v>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1166,10 +1169,13 @@
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1178,7 +1184,14 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -1188,31 +1201,35 @@
       <c r="A23" s="12"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
         <v>4</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E26" s="9">
         <v>3</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F26" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E28" s="8">
         <v>4</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F28" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>